<commit_message>
TP#20088: Getting FedEx integration tests to run with latest code base.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Freight Intl.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Freight Intl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwinchester\Documents\ShipWorks3x\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ShipWorks\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,13 +18,13 @@
     <definedName name="_lu1">#REF!</definedName>
     <definedName name="_lu2">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="142">
   <si>
     <t>FEDEX BUSINESS</t>
   </si>
@@ -321,10 +321,6 @@
   </si>
   <si>
     <t>ProcessShipmentRequest.RequestedShipment.Recipient.Address</t>
-  </si>
-  <si>
-    <t>Freight 
-International</t>
   </si>
   <si>
     <t>ProcessShipmentRequest.RequestedShipment.ShippingChargesPayment.Payor.ResponsibleParty</t>
@@ -459,8 +455,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="30" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -610,13 +606,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF7030A0"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -689,7 +678,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -847,32 +836,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1244,12 +1207,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -1260,9 +1223,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
@@ -1353,7 +1316,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1374,7 +1337,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
@@ -1383,7 +1346,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1397,7 +1360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1407,13 +1370,13 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1425,25 +1388,25 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1455,32 +1418,32 @@
     <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="14" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="12" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1490,21 +1453,21 @@
     <xf numFmtId="0" fontId="22" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="20" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="18" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1519,28 +1482,22 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2012,23 +1969,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2064,23 +2004,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2260,7 +2183,7 @@
   <sheetPr codeName="Sheet14">
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:EP12"/>
+  <dimension ref="A1:EO12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2271,51 +2194,52 @@
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="3"/>
-    <col min="2" max="2" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.5703125" style="4" customWidth="1"/>
-    <col min="6" max="9" width="20.7109375" style="4"/>
-    <col min="10" max="10" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="29" width="20.7109375" style="4"/>
-    <col min="30" max="30" width="27.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="50" width="20.7109375" style="4"/>
-    <col min="51" max="51" width="34" style="4" bestFit="1" customWidth="1"/>
-    <col min="52" max="68" width="20.7109375" style="4"/>
-    <col min="69" max="74" width="22.140625" style="4" customWidth="1"/>
-    <col min="75" max="75" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="25.5703125" style="4" customWidth="1"/>
-    <col min="77" max="87" width="22.140625" style="4" customWidth="1"/>
-    <col min="88" max="88" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="43" style="4" bestFit="1" customWidth="1"/>
-    <col min="90" max="91" width="20.7109375" style="4"/>
-    <col min="92" max="92" width="30.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="93" max="101" width="20.7109375" style="4"/>
-    <col min="102" max="102" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="103" max="115" width="20.7109375" style="4"/>
-    <col min="116" max="16384" width="20.7109375" style="3"/>
+    <col min="2" max="2" width="15.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" style="4" customWidth="1"/>
+    <col min="5" max="8" width="20.7109375" style="4"/>
+    <col min="9" max="9" width="36.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="28" width="20.7109375" style="4"/>
+    <col min="29" max="29" width="27.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="49" width="20.7109375" style="4"/>
+    <col min="50" max="50" width="34" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="67" width="20.7109375" style="4"/>
+    <col min="68" max="73" width="22.140625" style="4" customWidth="1"/>
+    <col min="74" max="74" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="25.5703125" style="4" customWidth="1"/>
+    <col min="76" max="86" width="22.140625" style="4" customWidth="1"/>
+    <col min="87" max="87" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="43" style="4" bestFit="1" customWidth="1"/>
+    <col min="89" max="90" width="20.7109375" style="4"/>
+    <col min="91" max="91" width="30.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="92" max="100" width="20.7109375" style="4"/>
+    <col min="101" max="101" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="102" max="114" width="20.7109375" style="4"/>
+    <col min="115" max="16384" width="20.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:146" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:146" s="17" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:145" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:145" s="17" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="C2" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="D2" s="14" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="G2" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="19" t="s">
@@ -2324,29 +2248,29 @@
       <c r="J2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="19" t="s">
-        <v>39</v>
+      <c r="K2" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="L2" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="M2" s="27" t="s">
-        <v>93</v>
+      <c r="M2" s="19" t="s">
+        <v>140</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="P2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="19" t="s">
         <v>69</v>
       </c>
       <c r="Q2" s="19" t="s">
         <v>69</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="S2" s="19" t="s">
         <v>97</v>
@@ -2360,22 +2284,22 @@
       <c r="V2" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="W2" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="X2" s="14" t="s">
+      <c r="W2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="19" t="s">
         <v>40</v>
       </c>
       <c r="Y2" s="19" t="s">
         <v>40</v>
       </c>
       <c r="Z2" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AA2" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB2" s="19" t="s">
         <v>98</v>
       </c>
       <c r="AC2" s="19" t="s">
@@ -2385,25 +2309,25 @@
         <v>98</v>
       </c>
       <c r="AE2" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AF2" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AG2" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH2" s="19" t="s">
         <v>100</v>
       </c>
       <c r="AI2" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ2" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ2" s="14" t="s">
         <v>120</v>
       </c>
       <c r="AK2" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AL2" s="14" t="s">
         <v>121</v>
@@ -2415,16 +2339,16 @@
         <v>123</v>
       </c>
       <c r="AO2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AP2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AQ2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="AR2" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="AP2" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AQ2" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AR2" s="14" t="s">
-        <v>120</v>
       </c>
       <c r="AS2" s="14" t="s">
         <v>125</v>
@@ -2433,40 +2357,40 @@
         <v>126</v>
       </c>
       <c r="AU2" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AV2" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="AV2" s="14" t="s">
-        <v>125</v>
-      </c>
       <c r="AW2" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AX2" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AY2" s="14" t="s">
         <v>128</v>
       </c>
       <c r="AZ2" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="BA2" s="14" t="s">
         <v>129</v>
       </c>
       <c r="BB2" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="BC2" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="BD2" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="BE2" s="14" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="BF2" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BG2" s="14" t="s">
         <v>104</v>
@@ -2481,19 +2405,19 @@
         <v>107</v>
       </c>
       <c r="BK2" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="BL2" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="BL2" s="14" t="s">
-        <v>131</v>
-      </c>
       <c r="BM2" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="BN2" s="14" t="s">
         <v>109</v>
       </c>
       <c r="BO2" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="BP2" s="14" t="s">
         <v>110</v>
@@ -2502,86 +2426,84 @@
         <v>111</v>
       </c>
       <c r="BR2" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BS2" s="14" t="s">
         <v>112</v>
       </c>
       <c r="BT2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="BU2" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="BV2" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="BU2" s="14" t="s">
+      <c r="BW2" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="BV2" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="BW2" s="14" t="s">
+      <c r="BX2" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="BX2" s="14" t="s">
+      <c r="BZ2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="BY2" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="BZ2" s="14" t="s">
-        <v>115</v>
-      </c>
       <c r="CA2" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="CB2" s="14" t="s">
         <v>115</v>
       </c>
       <c r="CC2" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="CD2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="CE2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="CF2" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="CD2" s="14" t="s">
+      <c r="CG2" s="14" t="s">
         <v>116</v>
-      </c>
-      <c r="CE2" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="CF2" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="CG2" s="14" t="s">
-        <v>117</v>
       </c>
       <c r="CH2" s="14" t="s">
         <v>117</v>
       </c>
       <c r="CI2" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="CJ2" s="14" t="s">
         <v>118</v>
       </c>
       <c r="CK2" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="CL2" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="CM2" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="CN2" s="14" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="CO2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="CP2" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="CP2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="CQ2" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="CR2" s="15" t="s">
-        <v>103</v>
-      </c>
+      <c r="CQ2" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="CR2" s="16"/>
       <c r="CS2" s="16"/>
       <c r="CT2" s="16"/>
       <c r="CU2" s="16"/>
@@ -2596,340 +2518,338 @@
       <c r="DD2" s="16"/>
       <c r="DE2" s="16"/>
       <c r="DF2" s="16"/>
-      <c r="DG2" s="16"/>
     </row>
-    <row r="3" spans="1:146" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:145" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="5" t="s">
         <v>68</v>
       </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="G3" s="39" t="s">
         <v>38</v>
       </c>
+      <c r="H3" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="I3" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AY3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="AZ3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="BA3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="BC3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="BE3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="BG3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="BH3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="BI3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="BJ3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="BK3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="BM3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AQ3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AS3" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AT3" s="6" t="s">
+      <c r="BN3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AU3" s="6" t="s">
+      <c r="BO3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AV3" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AX3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="AY3" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="AZ3" s="6" t="s">
+      <c r="BP3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="BQ3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="BR3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="BS3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="BT3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="BU3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BV3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="BW3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="BX3" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="BY3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BZ3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="CA3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="CB3" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="BA3" s="6" t="s">
+      <c r="CC3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="BB3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="BC3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="BD3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="BE3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="BF3" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="BG3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="BH3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="BI3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="BJ3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="BK3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="BL3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="BM3" s="12" t="s">
+      <c r="CD3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="CE3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CF3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="BN3" s="12" t="s">
+      <c r="CG3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="BO3" s="12" t="s">
+      <c r="CH3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="BP3" s="12" t="s">
+      <c r="CI3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="BQ3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="BR3" s="12" t="s">
+      <c r="CJ3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="CK3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="CL3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="CM3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="CN3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="CO3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="CP3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="CQ3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="BS3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="BT3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="BU3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="BV3" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="BW3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="BX3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="BY3" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="BZ3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="CA3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="CB3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="CC3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="CD3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="CE3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="CF3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="CG3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="CH3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="CI3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="CJ3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="CK3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="CL3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="CM3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="CN3" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="CO3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="CP3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="CQ3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="CR3" s="8" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="4" spans="1:146" s="43" customFormat="1" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:145" s="43" customFormat="1" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="b">
         <v>0</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="C4" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="30" t="s">
-        <v>137</v>
+      <c r="D4" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>18</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="26" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="26">
+      <c r="L4" s="26">
         <v>150</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="26">
+      <c r="N4" s="26">
         <v>2560</v>
       </c>
+      <c r="O4" s="26" t="s">
+        <v>17</v>
+      </c>
       <c r="P4" s="26" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R4" s="26" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="S4" s="26" t="s">
         <v>132</v>
@@ -2937,59 +2857,59 @@
       <c r="T4" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="U4" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="V4" s="26">
+      <c r="U4" s="26">
         <v>72601</v>
       </c>
+      <c r="V4" s="26" t="s">
+        <v>7</v>
+      </c>
       <c r="W4" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y4" s="26">
+        <v>1234567890</v>
+      </c>
+      <c r="Z4" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA4" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB4" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC4" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD4" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE4" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF4" s="26">
+        <v>150067600</v>
+      </c>
+      <c r="AG4" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y4" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z4" s="26">
-        <v>1234567890</v>
-      </c>
-      <c r="AA4" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB4" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC4" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD4" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF4" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG4" s="26">
-        <v>150067600</v>
-      </c>
-      <c r="AH4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJ4" s="26">
+      <c r="AI4" s="26">
         <v>630081440</v>
       </c>
+      <c r="AJ4" s="26" t="s">
+        <v>75</v>
+      </c>
       <c r="AK4" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AL4" s="26" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="AM4" s="26" t="s">
         <v>132</v>
@@ -2997,44 +2917,44 @@
       <c r="AN4" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="AO4" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="AP4" s="26">
+      <c r="AO4" s="26">
         <v>72601</v>
       </c>
+      <c r="AP4" s="26" t="s">
+        <v>7</v>
+      </c>
       <c r="AQ4" s="26" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="AR4" s="26" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="AS4" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT4" s="26" t="s">
         <v>8</v>
       </c>
+      <c r="AT4" s="26">
+        <v>2560</v>
+      </c>
       <c r="AU4" s="26">
-        <v>2560</v>
-      </c>
-      <c r="AV4" s="26">
         <v>1</v>
       </c>
+      <c r="AV4" s="26" t="s">
+        <v>138</v>
+      </c>
       <c r="AW4" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="AX4" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="AY4" s="26">
+      <c r="AX4" s="26">
         <v>1</v>
       </c>
-      <c r="AZ4" s="26" t="s">
+      <c r="AY4" s="26" t="s">
         <v>58</v>
       </c>
+      <c r="AZ4" s="26">
+        <v>150</v>
+      </c>
       <c r="BA4" s="26">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="BB4" s="26">
         <v>90</v>
@@ -3042,127 +2962,125 @@
       <c r="BC4" s="26">
         <v>90</v>
       </c>
-      <c r="BD4" s="26">
-        <v>90</v>
+      <c r="BD4" s="26" t="s">
+        <v>23</v>
       </c>
       <c r="BE4" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="BF4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="BG4" s="26">
+      <c r="BF4" s="26">
         <v>12345678</v>
       </c>
-      <c r="BH4" s="26" t="s">
+      <c r="BG4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="BI4" s="26">
+      <c r="BH4" s="26">
         <v>150067600</v>
       </c>
-      <c r="BJ4" s="26"/>
+      <c r="BI4" s="26"/>
+      <c r="BJ4" s="26" t="s">
+        <v>7</v>
+      </c>
       <c r="BK4" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM4" s="26">
+        <v>2560</v>
+      </c>
+      <c r="BN4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO4" s="26">
+        <v>200</v>
+      </c>
+      <c r="BP4" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="BR4" s="26">
+        <v>100</v>
+      </c>
+      <c r="BS4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="BT4" s="26">
+        <v>25</v>
+      </c>
+      <c r="BU4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="BV4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW4" s="26">
+        <v>123456789</v>
+      </c>
+      <c r="BX4" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="BY4" s="26">
+        <v>1</v>
+      </c>
+      <c r="BZ4" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="CA4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="BL4" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="BM4" s="26" t="s">
+      <c r="CB4" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="CC4" s="26">
+        <v>150</v>
+      </c>
+      <c r="CD4" s="26">
+        <v>1</v>
+      </c>
+      <c r="CE4" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="CF4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="BN4" s="26">
+      <c r="CG4" s="26">
         <v>2560</v>
       </c>
-      <c r="BO4" s="26" t="s">
+      <c r="CH4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="BP4" s="26">
-        <v>200</v>
-      </c>
-      <c r="BQ4" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="BR4" s="26" t="s">
+      <c r="CI4" s="26">
+        <v>2560</v>
+      </c>
+      <c r="CJ4" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="CK4" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="CL4" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="CM4" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="CN4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="CO4" s="26">
+        <v>1</v>
+      </c>
+      <c r="CP4" s="26">
+        <v>2560</v>
+      </c>
+      <c r="CQ4" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="BS4" s="26">
-        <v>100</v>
-      </c>
-      <c r="BT4" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="BU4" s="26">
-        <v>25</v>
-      </c>
-      <c r="BV4" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="BW4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="BX4" s="26">
-        <v>123456789</v>
-      </c>
-      <c r="BY4" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="BZ4" s="26">
-        <v>1</v>
-      </c>
-      <c r="CA4" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="CB4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="CC4" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="CD4" s="26">
-        <v>150</v>
-      </c>
-      <c r="CE4" s="26">
-        <v>1</v>
-      </c>
-      <c r="CF4" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="CG4" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="CH4" s="26">
-        <v>2560</v>
-      </c>
-      <c r="CI4" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="CJ4" s="26">
-        <v>2560</v>
-      </c>
-      <c r="CK4" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="CL4" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="CM4" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="CN4" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="CO4" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="CP4" s="26">
-        <v>1</v>
-      </c>
-      <c r="CQ4" s="26">
-        <v>2560</v>
-      </c>
-      <c r="CR4" s="33" t="s">
-        <v>8</v>
-      </c>
+      <c r="CR4" s="44"/>
       <c r="CS4" s="44"/>
       <c r="CT4" s="44"/>
       <c r="CU4" s="44"/>
@@ -3177,56 +3095,57 @@
       <c r="DD4" s="44"/>
       <c r="DE4" s="44"/>
       <c r="DF4" s="44"/>
-      <c r="DG4" s="44"/>
     </row>
-    <row r="5" spans="1:146" s="9" customFormat="1" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:145" s="9" customFormat="1" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="b">
         <v>0</v>
       </c>
       <c r="B5" s="48"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="34" t="s">
+      <c r="C5" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>138</v>
+      <c r="D5" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="H5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="I5" s="10" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="L5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="10">
+      <c r="L5" s="10">
         <v>150</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="10">
+      <c r="N5" s="10">
         <v>2560</v>
       </c>
+      <c r="O5" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="P5" s="10" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R5" s="10" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="S5" s="10" t="s">
         <v>132</v>
@@ -3234,59 +3153,59 @@
       <c r="T5" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="V5" s="10">
+      <c r="U5" s="10">
         <v>72601</v>
       </c>
+      <c r="V5" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="W5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y5" s="10">
+        <v>1234567890</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF5" s="10">
+        <v>150067600</v>
+      </c>
+      <c r="AG5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="X5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y5" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z5" s="10">
-        <v>1234567890</v>
-      </c>
-      <c r="AA5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG5" s="10">
-        <v>150067600</v>
-      </c>
-      <c r="AH5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJ5" s="10">
+      <c r="AI5" s="10">
         <v>630081440</v>
       </c>
+      <c r="AJ5" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="AK5" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AL5" s="10" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="AM5" s="10" t="s">
         <v>132</v>
@@ -3294,44 +3213,44 @@
       <c r="AN5" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="AO5" s="10" t="s">
+      <c r="AO5" s="10">
+        <v>72601</v>
+      </c>
+      <c r="AP5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ5" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT5" s="10">
+        <v>2560</v>
+      </c>
+      <c r="AU5" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="AW5" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="AP5" s="10">
-        <v>72601</v>
-      </c>
-      <c r="AQ5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AR5" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="AS5" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU5" s="10">
-        <v>2560</v>
-      </c>
-      <c r="AV5" s="10">
+      <c r="AX5" s="10">
         <v>1</v>
       </c>
-      <c r="AW5" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="AX5" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="AY5" s="10">
-        <v>1</v>
-      </c>
-      <c r="AZ5" s="10" t="s">
+      <c r="AY5" s="10" t="s">
         <v>58</v>
       </c>
+      <c r="AZ5" s="10">
+        <v>150</v>
+      </c>
       <c r="BA5" s="10">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="BB5" s="10">
         <v>90</v>
@@ -3339,127 +3258,125 @@
       <c r="BC5" s="10">
         <v>90</v>
       </c>
-      <c r="BD5" s="10">
-        <v>90</v>
+      <c r="BD5" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="BE5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BF5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="BG5" s="10">
+      <c r="BF5" s="10">
         <v>12345678</v>
       </c>
-      <c r="BH5" s="10" t="s">
+      <c r="BG5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="BI5" s="10">
+      <c r="BH5" s="10">
         <v>150067600</v>
       </c>
-      <c r="BJ5" s="10"/>
+      <c r="BI5" s="10"/>
+      <c r="BJ5" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="BK5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM5" s="10">
+        <v>2560</v>
+      </c>
+      <c r="BN5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO5" s="10">
+        <v>50</v>
+      </c>
+      <c r="BP5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="BR5" s="10">
+        <v>100</v>
+      </c>
+      <c r="BS5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="BT5" s="10">
+        <v>25</v>
+      </c>
+      <c r="BU5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="BV5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW5" s="10">
+        <v>123456789</v>
+      </c>
+      <c r="BX5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="BY5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BZ5" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="CA5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="BL5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="BM5" s="10" t="s">
+      <c r="CB5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="CC5" s="10">
+        <v>150</v>
+      </c>
+      <c r="CD5" s="10">
+        <v>1</v>
+      </c>
+      <c r="CE5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="CF5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="BN5" s="10">
+      <c r="CG5" s="10">
         <v>2560</v>
       </c>
-      <c r="BO5" s="10" t="s">
+      <c r="CH5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="BP5" s="10">
-        <v>50</v>
-      </c>
-      <c r="BQ5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="BR5" s="10" t="s">
+      <c r="CI5" s="10">
+        <v>2560</v>
+      </c>
+      <c r="CJ5" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="CK5" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="CL5" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="CM5" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="CN5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="CO5" s="10">
+        <v>1</v>
+      </c>
+      <c r="CP5" s="10">
+        <v>2560</v>
+      </c>
+      <c r="CQ5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="BS5" s="10">
-        <v>100</v>
-      </c>
-      <c r="BT5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="BU5" s="10">
-        <v>25</v>
-      </c>
-      <c r="BV5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="BW5" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="BX5" s="10">
-        <v>123456789</v>
-      </c>
-      <c r="BY5" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="BZ5" s="10">
-        <v>1</v>
-      </c>
-      <c r="CA5" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="CB5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="CC5" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="CD5" s="10">
-        <v>150</v>
-      </c>
-      <c r="CE5" s="10">
-        <v>1</v>
-      </c>
-      <c r="CF5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="CG5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="CH5" s="10">
-        <v>2560</v>
-      </c>
-      <c r="CI5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="CJ5" s="10">
-        <v>2560</v>
-      </c>
-      <c r="CK5" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="CL5" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="CM5" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="CN5" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="CO5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="CP5" s="10">
-        <v>1</v>
-      </c>
-      <c r="CQ5" s="10">
-        <v>2560</v>
-      </c>
-      <c r="CR5" s="11" t="s">
-        <v>8</v>
-      </c>
+      <c r="CR5" s="37"/>
       <c r="CS5" s="37"/>
       <c r="CT5" s="37"/>
       <c r="CU5" s="37"/>
@@ -3474,12 +3391,11 @@
       <c r="DD5" s="37"/>
       <c r="DE5" s="37"/>
       <c r="DF5" s="37"/>
-      <c r="DG5" s="37"/>
     </row>
-    <row r="6" spans="1:146" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:145" s="9" customFormat="1" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -3572,7 +3488,7 @@
       <c r="CO6" s="4"/>
       <c r="CP6" s="4"/>
       <c r="CQ6" s="4"/>
-      <c r="CR6" s="4"/>
+      <c r="CR6" s="37"/>
       <c r="CS6" s="37"/>
       <c r="CT6" s="37"/>
       <c r="CU6" s="37"/>
@@ -3587,12 +3503,11 @@
       <c r="DD6" s="37"/>
       <c r="DE6" s="37"/>
       <c r="DF6" s="37"/>
-      <c r="DG6" s="37"/>
     </row>
-    <row r="7" spans="1:146" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:145" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -3685,7 +3600,7 @@
       <c r="CO7" s="4"/>
       <c r="CP7" s="4"/>
       <c r="CQ7" s="4"/>
-      <c r="CR7" s="4"/>
+      <c r="CR7" s="37"/>
       <c r="CS7" s="37"/>
       <c r="CT7" s="37"/>
       <c r="CU7" s="37"/>
@@ -3700,9 +3615,9 @@
       <c r="DD7" s="37"/>
       <c r="DE7" s="37"/>
       <c r="DF7" s="37"/>
-      <c r="DG7" s="37"/>
     </row>
-    <row r="8" spans="1:146" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:145" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="CR8" s="3"/>
       <c r="CS8" s="3"/>
       <c r="CT8" s="3"/>
       <c r="CU8" s="3"/>
@@ -3721,12 +3636,11 @@
       <c r="DH8" s="3"/>
       <c r="DI8" s="3"/>
       <c r="DJ8" s="3"/>
-      <c r="DK8" s="3"/>
     </row>
-    <row r="9" spans="1:146" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:145" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -3819,7 +3733,7 @@
       <c r="CO9" s="4"/>
       <c r="CP9" s="4"/>
       <c r="CQ9" s="4"/>
-      <c r="CR9" s="4"/>
+      <c r="CR9" s="17"/>
       <c r="CS9" s="17"/>
       <c r="CT9" s="17"/>
       <c r="CU9" s="17"/>
@@ -3839,7 +3753,7 @@
       <c r="DI9" s="17"/>
       <c r="DJ9" s="17"/>
       <c r="DK9" s="17"/>
-      <c r="DL9" s="17"/>
+      <c r="DL9" s="16"/>
       <c r="DM9" s="16"/>
       <c r="DN9" s="16"/>
       <c r="DO9" s="16"/>
@@ -3850,7 +3764,7 @@
       <c r="DT9" s="16"/>
       <c r="DU9" s="16"/>
       <c r="DV9" s="16"/>
-      <c r="DW9" s="16"/>
+      <c r="DW9" s="24"/>
       <c r="DX9" s="24"/>
       <c r="DY9" s="24"/>
       <c r="DZ9" s="24"/>
@@ -3869,12 +3783,11 @@
       <c r="EM9" s="24"/>
       <c r="EN9" s="24"/>
       <c r="EO9" s="24"/>
-      <c r="EP9" s="24"/>
     </row>
-    <row r="10" spans="1:146" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:145" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -3967,7 +3880,7 @@
       <c r="CO10" s="4"/>
       <c r="CP10" s="4"/>
       <c r="CQ10" s="4"/>
-      <c r="CR10" s="4"/>
+      <c r="CR10" s="2"/>
       <c r="CS10" s="2"/>
       <c r="CT10" s="2"/>
       <c r="CU10" s="2"/>
@@ -3987,7 +3900,7 @@
       <c r="DI10" s="2"/>
       <c r="DJ10" s="2"/>
       <c r="DK10" s="2"/>
-      <c r="DL10" s="2"/>
+      <c r="DL10" s="40"/>
       <c r="DM10" s="40"/>
       <c r="DN10" s="40"/>
       <c r="DO10" s="40"/>
@@ -3995,15 +3908,14 @@
       <c r="DQ10" s="40"/>
       <c r="DR10" s="40"/>
       <c r="DS10" s="40"/>
-      <c r="DT10" s="40"/>
+      <c r="DT10" s="2"/>
       <c r="DU10" s="2"/>
       <c r="DV10" s="2"/>
-      <c r="DW10" s="2"/>
     </row>
-    <row r="11" spans="1:146" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:145" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -4096,7 +4008,7 @@
       <c r="CO11" s="4"/>
       <c r="CP11" s="4"/>
       <c r="CQ11" s="4"/>
-      <c r="CR11" s="4"/>
+      <c r="CR11" s="9"/>
       <c r="CS11" s="9"/>
       <c r="CT11" s="9"/>
       <c r="CU11" s="9"/>
@@ -4116,18 +4028,18 @@
       <c r="DI11" s="9"/>
       <c r="DJ11" s="9"/>
       <c r="DK11" s="9"/>
-      <c r="DL11" s="9"/>
-      <c r="DM11" s="41"/>
+      <c r="DL11" s="41"/>
+      <c r="DM11" s="42"/>
       <c r="DN11" s="42"/>
       <c r="DO11" s="42"/>
       <c r="DP11" s="42"/>
       <c r="DQ11" s="42"/>
       <c r="DR11" s="42"/>
       <c r="DS11" s="42"/>
-      <c r="DT11" s="42"/>
+      <c r="DT11" s="37"/>
       <c r="DU11" s="37"/>
       <c r="DV11" s="37"/>
-      <c r="DW11" s="37"/>
+      <c r="DW11" s="25"/>
       <c r="DX11" s="25"/>
       <c r="DY11" s="25"/>
       <c r="DZ11" s="25"/>
@@ -4146,12 +4058,11 @@
       <c r="EM11" s="25"/>
       <c r="EN11" s="25"/>
       <c r="EO11" s="25"/>
-      <c r="EP11" s="25"/>
     </row>
-    <row r="12" spans="1:146" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:145" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -4244,7 +4155,7 @@
       <c r="CO12" s="4"/>
       <c r="CP12" s="4"/>
       <c r="CQ12" s="4"/>
-      <c r="CR12" s="4"/>
+      <c r="CR12" s="9"/>
       <c r="CS12" s="9"/>
       <c r="CT12" s="9"/>
       <c r="CU12" s="9"/>
@@ -4264,18 +4175,18 @@
       <c r="DI12" s="9"/>
       <c r="DJ12" s="9"/>
       <c r="DK12" s="9"/>
-      <c r="DL12" s="9"/>
-      <c r="DM12" s="41"/>
+      <c r="DL12" s="41"/>
+      <c r="DM12" s="42"/>
       <c r="DN12" s="42"/>
       <c r="DO12" s="42"/>
       <c r="DP12" s="42"/>
       <c r="DQ12" s="42"/>
       <c r="DR12" s="42"/>
       <c r="DS12" s="42"/>
-      <c r="DT12" s="42"/>
+      <c r="DT12" s="37"/>
       <c r="DU12" s="37"/>
       <c r="DV12" s="37"/>
-      <c r="DW12" s="37"/>
+      <c r="DW12" s="25"/>
       <c r="DX12" s="25"/>
       <c r="DY12" s="25"/>
       <c r="DZ12" s="25"/>
@@ -4294,12 +4205,10 @@
       <c r="EM12" s="25"/>
       <c r="EN12" s="25"/>
       <c r="EO12" s="25"/>
-      <c r="EP12" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>